<commit_message>
Enhancement to report code snippet to show test steps count
</commit_message>
<xml_diff>
--- a/Omnius Test Case Document.xlsx
+++ b/Omnius Test Case Document.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhushana/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhushana/DocumentExplorerAssignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528D751E-33E8-8D4C-BAAA-10BF60064730}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB89471-0146-934C-BA6F-02327AD4E64D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="25440" windowHeight="14680" xr2:uid="{6F46BB43-1DBC-6E40-9168-7A15850DEC7F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="134">
   <si>
     <t>Project Name</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>User should be able to see uploading status of a document at top of Document section</t>
+  </si>
+  <si>
+    <t>Cannot be Automated</t>
+  </si>
+  <si>
+    <t>Can be Automated</t>
   </si>
 </sst>
 </file>
@@ -887,7 +893,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -901,7 +907,7 @@
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
     <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
@@ -1085,7 +1091,9 @@
         <v>35</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="6"/>
+      <c r="J11" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1116,7 +1124,9 @@
         <v>35</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="6"/>
+      <c r="J12" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1180,7 +1190,9 @@
         <v>29</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1211,7 +1223,9 @@
         <v>53</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -1242,7 +1256,9 @@
         <v>58</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -1438,7 +1454,9 @@
         <v>92</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="6"/>
+      <c r="J22" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -1469,7 +1487,9 @@
         <v>98</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="6"/>
+      <c r="J23" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -1533,7 +1553,9 @@
         <v>108</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="6"/>
+      <c r="J25" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -1564,7 +1586,9 @@
         <v>113</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="6"/>
+      <c r="J26" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -1595,7 +1619,9 @@
         <v>117</v>
       </c>
       <c r="I27" s="4"/>
-      <c r="J27" s="6"/>
+      <c r="J27" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -1626,7 +1652,9 @@
         <v>121</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="6"/>
+      <c r="J28" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="119">
       <c r="A29" s="4" t="s">
@@ -1654,7 +1682,9 @@
         <v>126</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="6"/>
+      <c r="J29" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="136">
       <c r="A30" s="4" t="s">
@@ -1682,7 +1712,9 @@
         <v>131</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="6"/>
+      <c r="J30" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>